<commit_message>
Build site at 2022-10-10 16:07:07 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3229.xlsx
+++ b/assets/disciplinas/LOM3229.xlsx
@@ -121,15 +121,15 @@
     <t>Requisitos:</t>
   </si>
   <si>
-    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">LOB1021 -  Física IV  (Requisito)
 </t>
   </si>
   <si>
     <t xml:space="preserve">LOM3016 -  Introdução à  Ciência dos Materiais  (Requisito)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
 </t>
   </si>
 </sst>

</xml_diff>

<commit_message>
Build site at 2023-03-13 16:21:36 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3229.xlsx
+++ b/assets/disciplinas/LOM3229.xlsx
@@ -130,15 +130,15 @@
     <t>Requisitos:</t>
   </si>
   <si>
+    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOB1021 -  Física IV  (Requisito)
 </t>
   </si>
   <si>
     <t xml:space="preserve">LOM3016 -  Introdução à  Ciência dos Materiais  (Requisito)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
 </t>
   </si>
 </sst>

</xml_diff>

<commit_message>
Build site at 2023-03-31 16:17:46 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3229.xlsx
+++ b/assets/disciplinas/LOM3229.xlsx
@@ -130,15 +130,15 @@
     <t>Requisitos:</t>
   </si>
   <si>
-    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">LOB1021 -  Física IV  (Requisito)
 </t>
   </si>
   <si>
     <t xml:space="preserve">LOM3016 -  Introdução à  Ciência dos Materiais  (Requisito)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOM3246 -  Técnicas de Caracterização de Materiais  (Indicação de Conjunto)
 </t>
   </si>
 </sst>

</xml_diff>